<commit_message>
Getting some Google security errors (trying to find a work around)
</commit_message>
<xml_diff>
--- a/resources/Test Companies.xlsx
+++ b/resources/Test Companies.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>Company</t>
   </si>
@@ -55,6 +55,9 @@
     <t>Anderson</t>
   </si>
   <si>
+    <t>Sent</t>
+  </si>
+  <si>
     <t>Anderd84@my.erau.edu</t>
   </si>
   <si>
@@ -113,9 +116,6 @@
   </si>
   <si>
     <t>Patterson</t>
-  </si>
-  <si>
-    <t>Sent</t>
   </si>
   <si>
     <t>Patterw7@my.erau.edu</t>
@@ -572,88 +572,98 @@
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="E5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="E6" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="E7" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>34</v>
@@ -671,7 +681,7 @@
         <v>37</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>38</v>
@@ -686,7 +696,9 @@
         <v>40</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="E10" s="2" t="s">
         <v>41</v>
       </c>

</xml_diff>